<commit_message>
Atualização da base Presença
</commit_message>
<xml_diff>
--- a/Presença.xlsx
+++ b/Presença.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abilitytecnologiabrcom-my.sharepoint.com/personal/anderson_bortolamedi_abilitytecnologia_com_br/Documents/Bases_Controle_SC/Bases Consulta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abilitytecnologiabrcom-my.sharepoint.com/personal/daniel_oliveira_abilitytecnologia_com_br/Documents/PY/painel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13336" documentId="8_{75F398DA-7C2B-43A7-9B09-B9B9CDD195AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06A458E8-8767-4994-92F2-E83176F33203}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7C94C5B-1287-4158-8829-A6433C4EC08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{7D81E428-CC76-4789-8287-B75737980914}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7D81E428-CC76-4789-8287-B75737980914}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista Pendencia" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2313" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2459" uniqueCount="610">
   <si>
     <t>Afastado</t>
   </si>
@@ -1824,6 +1824,54 @@
   </si>
   <si>
     <t>ALISSON FELIPE ROCHA</t>
+  </si>
+  <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>FLORIANOPOLIS</t>
+  </si>
+  <si>
+    <t>PALHOCA</t>
+  </si>
+  <si>
+    <t>SAO JOSE</t>
+  </si>
+  <si>
+    <t>JOINVILLE</t>
+  </si>
+  <si>
+    <t>CHAPECO</t>
+  </si>
+  <si>
+    <t>CRICIUMA</t>
+  </si>
+  <si>
+    <t>ICARA</t>
+  </si>
+  <si>
+    <t>BLUMENAU</t>
+  </si>
+  <si>
+    <t>BALNEARIO CAMBORIU</t>
+  </si>
+  <si>
+    <t>ITAJAI</t>
+  </si>
+  <si>
+    <t>NAVEGANTES</t>
+  </si>
+  <si>
+    <t>LAGES</t>
+  </si>
+  <si>
+    <t>TUBARAO</t>
+  </si>
+  <si>
+    <t>RIO DO SUL</t>
+  </si>
+  <si>
+    <t>BRUSQUE</t>
   </si>
 </sst>
 </file>
@@ -2384,7 +2432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2766,6 +2814,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3425,10 +3474,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
-<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60F09CFF-606B-4DFA-8E96-95D70C274BA1}" name="Tabela1" displayName="Tabela1" ref="A1:P146" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="A1:P146" xr:uid="{60F09CFF-606B-4DFA-8E96-95D70C274BA1}"/>
@@ -3862,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F5666-1E05-4535-8F57-CA87DBD785F0}">
-  <dimension ref="A1:S146"/>
+  <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3878,20 +3923,22 @@
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="17" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="88" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="77" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="77" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" customWidth="1"/>
+    <col min="20" max="20" width="21" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="92" t="s">
         <v>14</v>
       </c>
@@ -3949,8 +3996,11 @@
       <c r="S1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="129" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
         <v>33</v>
       </c>
@@ -3995,8 +4045,11 @@
       <c r="R2" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
         <v>33</v>
       </c>
@@ -4041,8 +4094,11 @@
       <c r="R3" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>33</v>
       </c>
@@ -4089,8 +4145,11 @@
       <c r="R4" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>33</v>
       </c>
@@ -4137,8 +4196,11 @@
       <c r="R5" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>33</v>
       </c>
@@ -4185,8 +4247,11 @@
       <c r="R6" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>33</v>
       </c>
@@ -4233,8 +4298,11 @@
       <c r="R7" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>33</v>
       </c>
@@ -4281,8 +4349,11 @@
       <c r="R8" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>33</v>
       </c>
@@ -4327,8 +4398,11 @@
       <c r="R9" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
         <v>33</v>
       </c>
@@ -4373,8 +4447,11 @@
       <c r="R10" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>33</v>
       </c>
@@ -4421,8 +4498,11 @@
       <c r="R11" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>33</v>
       </c>
@@ -4467,8 +4547,11 @@
       <c r="R12" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>33</v>
       </c>
@@ -4513,8 +4596,11 @@
       <c r="R13" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>33</v>
       </c>
@@ -4561,8 +4647,11 @@
       <c r="R14" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>33</v>
       </c>
@@ -4609,8 +4698,11 @@
       <c r="R15" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="79" t="s">
         <v>33</v>
       </c>
@@ -4655,8 +4747,11 @@
       <c r="R16" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
         <v>33</v>
       </c>
@@ -4703,8 +4798,11 @@
       <c r="R17" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="79" t="s">
         <v>33</v>
       </c>
@@ -4751,8 +4849,11 @@
       <c r="R18" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="79" t="s">
         <v>33</v>
       </c>
@@ -4801,8 +4902,11 @@
       <c r="R19" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="79" t="s">
         <v>33</v>
       </c>
@@ -4849,8 +4953,11 @@
       <c r="R20" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="79" t="s">
         <v>33</v>
       </c>
@@ -4897,8 +5004,11 @@
       <c r="R21" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
         <v>33</v>
       </c>
@@ -4943,8 +5053,11 @@
       <c r="R22" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
         <v>33</v>
       </c>
@@ -4991,8 +5104,11 @@
       <c r="R23" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T23" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
         <v>33</v>
       </c>
@@ -5037,8 +5153,11 @@
       <c r="R24" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T24" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
         <v>33</v>
       </c>
@@ -5083,8 +5202,11 @@
       <c r="R25" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
         <v>33</v>
       </c>
@@ -5131,8 +5253,11 @@
       <c r="R26" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T26" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
         <v>33</v>
       </c>
@@ -5177,8 +5302,11 @@
       <c r="R27" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
         <v>33</v>
       </c>
@@ -5223,8 +5351,11 @@
       <c r="R28" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T28" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="79" t="s">
         <v>33</v>
       </c>
@@ -5271,8 +5402,11 @@
       <c r="R29" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T29" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="79" t="s">
         <v>33</v>
       </c>
@@ -5319,8 +5453,11 @@
       <c r="R30" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T30" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
         <v>33</v>
       </c>
@@ -5365,8 +5502,11 @@
       <c r="R31" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T31" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
         <v>33</v>
       </c>
@@ -5413,8 +5553,11 @@
       <c r="R32" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T32" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
         <v>33</v>
       </c>
@@ -5461,8 +5604,11 @@
       <c r="R33" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T33" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
         <v>33</v>
       </c>
@@ -5507,8 +5653,11 @@
       <c r="R34" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T34" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
         <v>33</v>
       </c>
@@ -5553,8 +5702,11 @@
       <c r="R35" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T35" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
         <v>33</v>
       </c>
@@ -5601,8 +5753,11 @@
       <c r="R36" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T36" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="79" t="s">
         <v>33</v>
       </c>
@@ -5647,8 +5802,11 @@
       <c r="R37" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T37" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="79" t="s">
         <v>33</v>
       </c>
@@ -5693,8 +5851,11 @@
       <c r="R38" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T38" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
         <v>33</v>
       </c>
@@ -5739,8 +5900,11 @@
       <c r="R39" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T39" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
         <v>33</v>
       </c>
@@ -5785,8 +5949,11 @@
       <c r="R40" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T40" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
         <v>33</v>
       </c>
@@ -5831,8 +5998,11 @@
       <c r="R41" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T41" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
         <v>33</v>
       </c>
@@ -5879,8 +6049,11 @@
       <c r="R42" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T42" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="79" t="s">
         <v>33</v>
       </c>
@@ -5925,8 +6098,11 @@
       <c r="R43" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="79" t="s">
         <v>33</v>
       </c>
@@ -5973,8 +6149,11 @@
       <c r="R44" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T44" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="79" t="s">
         <v>33</v>
       </c>
@@ -6019,8 +6198,11 @@
       <c r="R45" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T45" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="79" t="s">
         <v>33</v>
       </c>
@@ -6065,8 +6247,11 @@
       <c r="R46" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T46" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="79" t="s">
         <v>33</v>
       </c>
@@ -6113,8 +6298,11 @@
       <c r="R47" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T47" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="79" t="s">
         <v>33</v>
       </c>
@@ -6159,8 +6347,11 @@
       <c r="R48" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T48" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="79" t="s">
         <v>33</v>
       </c>
@@ -6207,8 +6398,11 @@
       <c r="R49" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T49" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="79" t="s">
         <v>33</v>
       </c>
@@ -6253,8 +6447,11 @@
       <c r="R50" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T50" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="79" t="s">
         <v>33</v>
       </c>
@@ -6301,8 +6498,11 @@
       <c r="R51" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T51" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="79" t="s">
         <v>33</v>
       </c>
@@ -6353,8 +6553,11 @@
       <c r="R52" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T52" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="79" t="s">
         <v>33</v>
       </c>
@@ -6401,8 +6604,11 @@
       <c r="R53" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T53" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="79" t="s">
         <v>33</v>
       </c>
@@ -6447,8 +6653,11 @@
       <c r="R54" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T54" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="79" t="s">
         <v>33</v>
       </c>
@@ -6493,8 +6702,11 @@
       <c r="R55" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T55" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="79" t="s">
         <v>33</v>
       </c>
@@ -6541,8 +6753,11 @@
       <c r="R56" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T56" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="79" t="s">
         <v>33</v>
       </c>
@@ -6593,8 +6808,11 @@
       <c r="R57" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T57" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="79" t="s">
         <v>33</v>
       </c>
@@ -6639,8 +6857,11 @@
       <c r="R58" s="82" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T58" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="79" t="s">
         <v>33</v>
       </c>
@@ -6685,8 +6906,11 @@
       <c r="R59" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T59" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="79" t="s">
         <v>33</v>
       </c>
@@ -6733,8 +6957,11 @@
       <c r="R60" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T60" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="79" t="s">
         <v>33</v>
       </c>
@@ -6785,8 +7012,11 @@
       <c r="R61" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T61" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="79" t="s">
         <v>33</v>
       </c>
@@ -6833,8 +7063,11 @@
       <c r="R62" s="82" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T62" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="79" t="s">
         <v>33</v>
       </c>
@@ -6879,8 +7112,11 @@
       <c r="R63" s="82" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T63" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="79" t="s">
         <v>33</v>
       </c>
@@ -6925,8 +7161,11 @@
       <c r="R64" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T64" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="79" t="s">
         <v>33</v>
       </c>
@@ -6975,8 +7214,11 @@
       <c r="R65" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T65" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="79" t="s">
         <v>33</v>
       </c>
@@ -7021,8 +7263,11 @@
       <c r="R66" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T66" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="79" t="s">
         <v>33</v>
       </c>
@@ -7067,8 +7312,11 @@
       <c r="R67" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T67" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="79" t="s">
         <v>33</v>
       </c>
@@ -7119,8 +7367,11 @@
       <c r="R68" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T68" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="79" t="s">
         <v>33</v>
       </c>
@@ -7167,8 +7418,11 @@
       <c r="R69" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T69" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="79" t="s">
         <v>33</v>
       </c>
@@ -7213,8 +7467,11 @@
       <c r="R70" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T70" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="79" t="s">
         <v>33</v>
       </c>
@@ -7259,8 +7516,11 @@
       <c r="R71" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T71" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="79" t="s">
         <v>33</v>
       </c>
@@ -7307,8 +7567,11 @@
       <c r="R72" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T72" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="79" t="s">
         <v>33</v>
       </c>
@@ -7353,8 +7616,11 @@
       <c r="R73" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T73" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="79" t="s">
         <v>33</v>
       </c>
@@ -7401,8 +7667,11 @@
       <c r="R74" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T74" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="79" t="s">
         <v>33</v>
       </c>
@@ -7447,8 +7716,11 @@
       <c r="R75" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T75" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="79" t="s">
         <v>33</v>
       </c>
@@ -7493,8 +7765,11 @@
       <c r="R76" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T76" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="79" t="s">
         <v>33</v>
       </c>
@@ -7539,8 +7814,11 @@
       <c r="R77" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T77" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="79" t="s">
         <v>33</v>
       </c>
@@ -7591,8 +7869,11 @@
       <c r="R78" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T78" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="79" t="s">
         <v>33</v>
       </c>
@@ -7637,8 +7918,11 @@
       <c r="R79" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T79" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="79" t="s">
         <v>33</v>
       </c>
@@ -7683,8 +7967,11 @@
       <c r="R80" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T80" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="79" t="s">
         <v>33</v>
       </c>
@@ -7729,8 +8016,11 @@
       <c r="R81" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T81" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="79" t="s">
         <v>33</v>
       </c>
@@ -7775,8 +8065,11 @@
       <c r="R82" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T82" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="79" t="s">
         <v>33</v>
       </c>
@@ -7821,8 +8114,11 @@
       <c r="R83" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T83" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="79" t="s">
         <v>33</v>
       </c>
@@ -7867,8 +8163,11 @@
       <c r="R84" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T84" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="79" t="s">
         <v>33</v>
       </c>
@@ -7913,8 +8212,11 @@
       <c r="R85" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T85" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="79" t="s">
         <v>33</v>
       </c>
@@ -7961,8 +8263,11 @@
       <c r="R86" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T86" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
         <v>33</v>
       </c>
@@ -8009,8 +8314,11 @@
       <c r="R87" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T87" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="79" t="s">
         <v>33</v>
       </c>
@@ -8057,8 +8365,11 @@
       <c r="R88" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T88" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="79" t="s">
         <v>33</v>
       </c>
@@ -8103,8 +8414,11 @@
       <c r="R89" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T89" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="79" t="s">
         <v>33</v>
       </c>
@@ -8151,8 +8465,11 @@
       <c r="R90" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T90" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="79" t="s">
         <v>33</v>
       </c>
@@ -8197,8 +8514,11 @@
       <c r="R91" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T91" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="79" t="s">
         <v>33</v>
       </c>
@@ -8245,8 +8565,11 @@
       <c r="R92" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T92" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="79" t="s">
         <v>33</v>
       </c>
@@ -8293,8 +8616,11 @@
       <c r="R93" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T93" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="79" t="s">
         <v>33</v>
       </c>
@@ -8339,8 +8665,11 @@
       <c r="R94" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T94" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="79" t="s">
         <v>33</v>
       </c>
@@ -8385,8 +8714,11 @@
       <c r="R95" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T95" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="79" t="s">
         <v>33</v>
       </c>
@@ -8433,8 +8765,11 @@
       <c r="R96" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T96" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="79" t="s">
         <v>33</v>
       </c>
@@ -8479,8 +8814,11 @@
       <c r="R97" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T97" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="79" t="s">
         <v>33</v>
       </c>
@@ -8527,8 +8865,11 @@
       <c r="R98" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T98" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="79" t="s">
         <v>33</v>
       </c>
@@ -8575,8 +8916,11 @@
       <c r="R99" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T99" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="79" t="s">
         <v>33</v>
       </c>
@@ -8621,8 +8965,11 @@
       <c r="R100" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T100" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="79" t="s">
         <v>33</v>
       </c>
@@ -8667,8 +9014,11 @@
       <c r="R101" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T101" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="79" t="s">
         <v>33</v>
       </c>
@@ -8715,8 +9065,11 @@
       <c r="R102" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T102" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="79" t="s">
         <v>33</v>
       </c>
@@ -8761,8 +9114,11 @@
       <c r="R103" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T103" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="79" t="s">
         <v>33</v>
       </c>
@@ -8809,8 +9165,11 @@
       <c r="R104" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T104" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="79" t="s">
         <v>33</v>
       </c>
@@ -8855,8 +9214,11 @@
       <c r="R105" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T105" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="79" t="s">
         <v>33</v>
       </c>
@@ -8901,8 +9263,11 @@
       <c r="R106" s="82" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T106" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="79" t="s">
         <v>33</v>
       </c>
@@ -8949,8 +9314,11 @@
       <c r="R107" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T107" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="79" t="s">
         <v>33</v>
       </c>
@@ -8989,8 +9357,11 @@
         <v>49</v>
       </c>
       <c r="P108" s="82"/>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T108" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="79" t="s">
         <v>33</v>
       </c>
@@ -9031,8 +9402,11 @@
         <v>41</v>
       </c>
       <c r="P109" s="82"/>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T109" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="79" t="s">
         <v>33</v>
       </c>
@@ -9073,8 +9447,11 @@
         <v>49</v>
       </c>
       <c r="P110" s="82"/>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T110" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="79" t="s">
         <v>33</v>
       </c>
@@ -9115,8 +9492,11 @@
         <v>41</v>
       </c>
       <c r="P111" s="82"/>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T111" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="79" t="s">
         <v>33</v>
       </c>
@@ -9157,8 +9537,11 @@
         <v>49</v>
       </c>
       <c r="P112" s="82"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T112" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="79" t="s">
         <v>33</v>
       </c>
@@ -9197,8 +9580,11 @@
         <v>41</v>
       </c>
       <c r="P113" s="82"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T113" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="79" t="s">
         <v>33</v>
       </c>
@@ -9239,8 +9625,11 @@
         <v>49</v>
       </c>
       <c r="P114" s="82"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T114" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="79" t="s">
         <v>33</v>
       </c>
@@ -9281,8 +9670,11 @@
         <v>49</v>
       </c>
       <c r="P115" s="82"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T115" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="79" t="s">
         <v>33</v>
       </c>
@@ -9323,8 +9715,11 @@
         <v>49</v>
       </c>
       <c r="P116" s="82"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T116" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="79" t="s">
         <v>33</v>
       </c>
@@ -9363,8 +9758,11 @@
         <v>49</v>
       </c>
       <c r="P117" s="82"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T117" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="79" t="s">
         <v>33</v>
       </c>
@@ -9403,8 +9801,11 @@
         <v>49</v>
       </c>
       <c r="P118" s="82"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T118" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="79" t="s">
         <v>33</v>
       </c>
@@ -9443,8 +9844,11 @@
         <v>41</v>
       </c>
       <c r="P119" s="82"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T119" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="79" t="s">
         <v>33</v>
       </c>
@@ -9485,8 +9889,11 @@
         <v>49</v>
       </c>
       <c r="P120" s="82"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T120" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="79" t="s">
         <v>33</v>
       </c>
@@ -9525,8 +9932,11 @@
         <v>41</v>
       </c>
       <c r="P121" s="82"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T121" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="79" t="s">
         <v>33</v>
       </c>
@@ -9567,8 +9977,11 @@
         <v>49</v>
       </c>
       <c r="P122" s="82"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T122" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="79" t="s">
         <v>33</v>
       </c>
@@ -9611,8 +10024,11 @@
         <v>49</v>
       </c>
       <c r="P123" s="82"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T123" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="79" t="s">
         <v>33</v>
       </c>
@@ -9651,8 +10067,11 @@
         <v>41</v>
       </c>
       <c r="P124" s="82"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T124" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="79" t="s">
         <v>33</v>
       </c>
@@ -9693,8 +10112,11 @@
         <v>49</v>
       </c>
       <c r="P125" s="82"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T125" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="79" t="s">
         <v>33</v>
       </c>
@@ -9733,8 +10155,11 @@
         <v>41</v>
       </c>
       <c r="P126" s="82"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T126" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="79" t="s">
         <v>33</v>
       </c>
@@ -9773,8 +10198,11 @@
         <v>41</v>
       </c>
       <c r="P127" s="82"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T127" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="79" t="s">
         <v>33</v>
       </c>
@@ -9817,8 +10245,11 @@
         <v>49</v>
       </c>
       <c r="P128" s="82"/>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T128" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="79" t="s">
         <v>33</v>
       </c>
@@ -9859,8 +10290,11 @@
         <v>49</v>
       </c>
       <c r="P129" s="82"/>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T129" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="79" t="s">
         <v>33</v>
       </c>
@@ -9905,8 +10339,11 @@
         <v>49</v>
       </c>
       <c r="P130" s="82"/>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T130" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="79" t="s">
         <v>33</v>
       </c>
@@ -9945,8 +10382,11 @@
         <v>41</v>
       </c>
       <c r="P131" s="82"/>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T131" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="79" t="s">
         <v>33</v>
       </c>
@@ -9991,8 +10431,11 @@
         <v>41</v>
       </c>
       <c r="P132" s="82"/>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T132" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="79" t="s">
         <v>33</v>
       </c>
@@ -10033,8 +10476,11 @@
         <v>41</v>
       </c>
       <c r="P133" s="82"/>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T133" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="79" t="s">
         <v>33</v>
       </c>
@@ -10079,8 +10525,11 @@
         <v>49</v>
       </c>
       <c r="P134" s="82"/>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T134" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="79" t="s">
         <v>33</v>
       </c>
@@ -10119,8 +10568,11 @@
         <v>49</v>
       </c>
       <c r="P135" s="82"/>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T135" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="79" t="s">
         <v>33</v>
       </c>
@@ -10163,8 +10615,11 @@
         <v>41</v>
       </c>
       <c r="P136" s="82"/>
-    </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T136" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="79" t="s">
         <v>33</v>
       </c>
@@ -10203,8 +10658,11 @@
         <v>49</v>
       </c>
       <c r="P137" s="82"/>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T137" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="79" t="s">
         <v>33</v>
       </c>
@@ -10245,8 +10703,11 @@
         <v>49</v>
       </c>
       <c r="P138" s="82"/>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T138" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="79" t="s">
         <v>33</v>
       </c>
@@ -10285,8 +10746,11 @@
         <v>41</v>
       </c>
       <c r="P139" s="82"/>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T139" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="79" t="s">
         <v>33</v>
       </c>
@@ -10327,8 +10791,11 @@
         <v>41</v>
       </c>
       <c r="P140" s="82"/>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T140" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="79" t="s">
         <v>33</v>
       </c>
@@ -10367,8 +10834,11 @@
         <v>41</v>
       </c>
       <c r="P141" s="82"/>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T141" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="79" t="s">
         <v>33</v>
       </c>
@@ -10409,8 +10879,11 @@
         <v>41</v>
       </c>
       <c r="P142" s="82"/>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T142" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="79" t="s">
         <v>33</v>
       </c>
@@ -10451,8 +10924,11 @@
         <v>41</v>
       </c>
       <c r="P143" s="82"/>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T143" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="79" t="s">
         <v>33</v>
       </c>
@@ -10491,8 +10967,11 @@
         <v>41</v>
       </c>
       <c r="P144" s="82"/>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T144" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="79" t="s">
         <v>33</v>
       </c>
@@ -10533,8 +11012,11 @@
         <v>41</v>
       </c>
       <c r="P145" s="82"/>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T145" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="125" t="s">
         <v>33</v>
       </c>
@@ -10575,6 +11057,9 @@
         <v>41</v>
       </c>
       <c r="P146" s="82"/>
+      <c r="T146" t="s">
+        <v>598</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -14786,7 +15271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B9220E-0AD4-48DC-AE9E-027B8C90F225}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -15772,6 +16257,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100926F1CD2B45B9C4C894002560E0BD142" ma:contentTypeVersion="1" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="f4a1b93fec6e716e2ca9abad63531a40">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2f9e23e-5e61-4470-9086-ebd7a1ce8bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c49c4701ea1cf54364ca03533ff3772" ns3:_="">
     <xsd:import namespace="f2f9e23e-5e61-4470-9086-ebd7a1ce8bdf"/>
@@ -15897,22 +16391,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664CD28B-78CD-4121-BD6B-F39B53791255}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36DBA938-95E5-4BDA-B51A-82531F644CAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15930,19 +16423,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00EB286D-7B66-4B58-8665-C13E847E4E32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664CD28B-78CD-4121-BD6B-F39B53791255}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>